<commit_message>
dev: update dependencies update: data
</commit_message>
<xml_diff>
--- a/data/accessory.xlsx
+++ b/data/accessory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\home\vick\dev\motleycrowd-service\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1657CDF7-5346-41A7-82DB-2BBD88B0A62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669CA3EC-62F8-46DA-8284-947125AA21B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="4630" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="badge" sheetId="1" r:id="rId1"/>
@@ -4524,7 +4524,7 @@
         <v>60</v>
       </c>
       <c r="C26" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>